<commit_message>
assignment 12 and 13
</commit_message>
<xml_diff>
--- a/Assignment_Details.xlsx
+++ b/Assignment_Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/52e1f49cefcf4ae0/Documents/GitHub/Apr22-Web-Fundamentals_Assignments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_F25DC773A252ABDACC104835C91E41EE5ADE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4F30E65-9CA0-4CE3-B7AF-F72866DFCB53}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_F25DC773A252ABDACC104835C91E41EE5ADE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{216C8521-29FB-4E9C-BAC3-ABF32BFFDB32}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t>Instructor</t>
   </si>
@@ -169,6 +169,15 @@
   </si>
   <si>
     <t>https://dilshaudayanperuvadathu.github.io/Apr22-Web-Fundamentals_Assignments/April/Week_4/Assignment_11/BoxWithImagePara.html</t>
+  </si>
+  <si>
+    <t>Abhishek Sir</t>
+  </si>
+  <si>
+    <t>Flex Box</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1iaP3v3sI6nc5-VYPDTHDJhddFuh_QfWa?usp=sharing</t>
   </si>
 </sst>
 </file>
@@ -513,6 +522,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>414342</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4141147</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1905000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1321A6D-B804-492A-8417-FDFDBB5A953C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4940622" y="15529561"/>
+          <a:ext cx="3726805" cy="1790699"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -779,10 +832,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.6640625" defaultRowHeight="15.6" thickTop="1" thickBottom="1" x14ac:dyDescent="0.35"/>
@@ -1010,8 +1063,39 @@
       <c r="E12" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="6" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="11">
+        <v>44678</v>
+      </c>
+      <c r="B13" s="10">
+        <v>12</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="158.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="11">
+        <v>44679</v>
+      </c>
+      <c r="B14" s="10">
+        <v>13</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1027,9 +1111,11 @@
     <hyperlink ref="F9" r:id="rId9" xr:uid="{566F3A78-FF8A-4856-A0E3-8FFB2B318D05}"/>
     <hyperlink ref="F10" r:id="rId10" xr:uid="{86258B6D-BEAE-4C86-B623-709EE2DAD377}"/>
     <hyperlink ref="F11" r:id="rId11" xr:uid="{4ED0C640-EBCD-4ED4-BFE6-395A429C4492}"/>
+    <hyperlink ref="E13" r:id="rId12" xr:uid="{90CEE922-E643-4712-BA30-2EB7F9E20897}"/>
+    <hyperlink ref="F12" r:id="rId13" xr:uid="{2DDD6D5C-A47F-4CD7-A660-38A07E12F1D3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
-  <drawing r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
+  <drawing r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>